<commit_message>
Removed some findings in line with email from emma.
</commit_message>
<xml_diff>
--- a/tabular/contributed/190408 VEL TABLE.xlsx
+++ b/tabular/contributed/190408 VEL TABLE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="49840" windowHeight="28340"/>
+    <workbookView xWindow="12440" yWindow="5340" windowWidth="47320" windowHeight="21240"/>
   </bookViews>
   <sheets>
     <sheet name="VEL" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1569" uniqueCount="154">
   <si>
     <t>in vivo</t>
   </si>
@@ -335,9 +335,6 @@
   </si>
   <si>
     <t>11.8</t>
-  </si>
-  <si>
-    <t>44K</t>
   </si>
   <si>
     <t>58S</t>
@@ -1007,11 +1004,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P123"/>
+  <dimension ref="A1:P121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G122" sqref="G122"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1036,46 +1033,46 @@
   <sheetData>
     <row r="1" spans="1:16" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="D1" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>142</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>143</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="8" t="s">
         <v>131</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>132</v>
       </c>
       <c r="O1" s="9" t="s">
         <v>3</v>
@@ -1135,13 +1132,13 @@
         <v>4</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>5</v>
@@ -1156,10 +1153,10 @@
         <v>5</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L3" s="12" t="s">
         <v>5</v>
@@ -1227,13 +1224,13 @@
         <v>4</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>5</v>
@@ -1248,16 +1245,16 @@
         <v>5</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L5" s="12" t="s">
         <v>5</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N5" s="22">
         <v>28564569</v>
@@ -1267,19 +1264,19 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>5</v>
@@ -1294,16 +1291,16 @@
         <v>5</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L6" s="12" t="s">
         <v>5</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N6" s="22">
         <v>28564569</v>
@@ -1313,19 +1310,19 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>5</v>
@@ -1340,16 +1337,16 @@
         <v>5</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L7" s="12" t="s">
         <v>5</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N7" s="22">
         <v>28564569</v>
@@ -1521,7 +1518,7 @@
         <v>2</v>
       </c>
       <c r="I11" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>5</v>
@@ -1628,7 +1625,7 @@
         <v>5</v>
       </c>
       <c r="N13" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O13" s="16"/>
       <c r="P13" s="17"/>
@@ -1720,7 +1717,7 @@
         <v>5</v>
       </c>
       <c r="N15" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O15" s="16"/>
       <c r="P15" s="17"/>
@@ -1920,10 +1917,10 @@
         <v>63</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F20" s="13" t="s">
         <v>5</v>
@@ -1938,10 +1935,10 @@
         <v>5</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K20" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L20" s="12" t="s">
         <v>5</v>
@@ -1996,7 +1993,7 @@
         <v>5</v>
       </c>
       <c r="N21" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O21" s="16"/>
       <c r="P21" s="17"/>
@@ -2150,10 +2147,10 @@
         <v>15</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F25" s="13" t="s">
         <v>5</v>
@@ -2171,7 +2168,7 @@
         <v>80</v>
       </c>
       <c r="K25" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L25" s="12" t="s">
         <v>5</v>
@@ -2196,10 +2193,10 @@
         <v>15</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F26" s="13" t="s">
         <v>5</v>
@@ -2217,7 +2214,7 @@
         <v>93</v>
       </c>
       <c r="K26" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L26" s="12" t="s">
         <v>5</v>
@@ -2242,10 +2239,10 @@
         <v>15</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F27" s="13" t="s">
         <v>5</v>
@@ -2260,10 +2257,10 @@
         <v>5</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K27" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L27" s="12" t="s">
         <v>5</v>
@@ -2288,10 +2285,10 @@
         <v>15</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F28" s="13" t="s">
         <v>5</v>
@@ -2306,10 +2303,10 @@
         <v>5</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K28" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L28" s="12" t="s">
         <v>5</v>
@@ -2364,7 +2361,7 @@
         <v>5</v>
       </c>
       <c r="N29" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O29" s="16"/>
       <c r="P29" s="17"/>
@@ -2462,38 +2459,38 @@
       <c r="P31" s="17"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A32" s="13" t="s">
-        <v>104</v>
+      <c r="A32" s="12" t="s">
+        <v>1</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="F32" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="G32" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H32" s="13" t="s">
-        <v>0</v>
+        <v>65</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>2</v>
       </c>
       <c r="I32" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="J32" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="K32" s="13" t="s">
-        <v>110</v>
+        <v>66</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K32" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="L32" s="12" t="s">
         <v>5</v>
@@ -2502,14 +2499,14 @@
         <v>5</v>
       </c>
       <c r="N32" s="22">
-        <v>28564569</v>
+        <v>27353271</v>
       </c>
       <c r="O32" s="19"/>
       <c r="P32" s="17"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A33" s="12" t="s">
-        <v>1</v>
+      <c r="A33" s="13" t="s">
+        <v>119</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>4</v>
@@ -2517,38 +2514,38 @@
       <c r="C33" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D33" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F33" s="12" t="s">
+      <c r="D33" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="F33" s="13" t="s">
         <v>5</v>
       </c>
       <c r="G33" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H33" s="12" t="s">
-        <v>2</v>
+      <c r="H33" s="13" t="s">
+        <v>0</v>
       </c>
       <c r="I33" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="J33" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="K33" s="12" t="s">
-        <v>5</v>
+        <v>85</v>
+      </c>
+      <c r="J33" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="K33" s="23" t="s">
+        <v>112</v>
       </c>
       <c r="L33" s="12" t="s">
         <v>5</v>
       </c>
       <c r="M33" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="N33" s="22">
-        <v>27353271</v>
+        <v>136</v>
+      </c>
+      <c r="N33" s="20">
+        <v>29221887</v>
       </c>
       <c r="O33" s="19"/>
       <c r="P33" s="17"/>
@@ -2564,10 +2561,10 @@
         <v>65</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F34" s="13" t="s">
         <v>5</v>
@@ -2585,13 +2582,13 @@
         <v>80</v>
       </c>
       <c r="K34" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L34" s="12" t="s">
         <v>5</v>
       </c>
       <c r="M34" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N34" s="20">
         <v>29221887</v>
@@ -2601,83 +2598,83 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="13" t="s">
-        <v>121</v>
+        <v>1</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E35" s="13" t="s">
         <v>134</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="G35" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="G35" s="13" t="s">
         <v>7</v>
       </c>
       <c r="H35" s="13" t="s">
         <v>0</v>
       </c>
       <c r="I35" s="21" t="s">
-        <v>85</v>
+        <v>5</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="K35" s="23" t="s">
-        <v>113</v>
+        <v>114</v>
+      </c>
+      <c r="K35" s="13" t="s">
+        <v>112</v>
       </c>
       <c r="L35" s="12" t="s">
         <v>5</v>
       </c>
       <c r="M35" s="12" t="s">
-        <v>137</v>
+        <v>5</v>
       </c>
       <c r="N35" s="20">
-        <v>29221887</v>
+        <v>26569658</v>
       </c>
       <c r="O35" s="19"/>
       <c r="P35" s="17"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="F36" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="G36" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H36" s="13" t="s">
-        <v>0</v>
+        <v>67</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>2</v>
       </c>
       <c r="I36" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="J36" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="K36" s="13" t="s">
-        <v>113</v>
+        <v>68</v>
+      </c>
+      <c r="J36" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K36" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="L36" s="12" t="s">
         <v>5</v>
@@ -2685,45 +2682,45 @@
       <c r="M36" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N36" s="20">
-        <v>26569658</v>
+      <c r="N36" s="22">
+        <v>27353271</v>
       </c>
       <c r="O36" s="19"/>
       <c r="P36" s="17"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A37" s="12" t="s">
+      <c r="A37" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F37" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G37" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H37" s="12" t="s">
-        <v>2</v>
+        <v>104</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>0</v>
       </c>
       <c r="I37" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="J37" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="K37" s="12" t="s">
-        <v>5</v>
+        <v>5</v>
+      </c>
+      <c r="J37" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="K37" s="13" t="s">
+        <v>109</v>
       </c>
       <c r="L37" s="12" t="s">
         <v>5</v>
@@ -2732,44 +2729,44 @@
         <v>5</v>
       </c>
       <c r="N37" s="22">
-        <v>27353271</v>
+        <v>28564569</v>
       </c>
       <c r="O37" s="19"/>
       <c r="P37" s="17"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A38" s="13" t="s">
-        <v>1</v>
+      <c r="A38" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="F38" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="G38" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H38" s="13" t="s">
-        <v>0</v>
+      <c r="C38" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" s="12" t="s">
+        <v>2</v>
       </c>
       <c r="I38" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="J38" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="K38" s="13" t="s">
-        <v>110</v>
+        <v>18</v>
+      </c>
+      <c r="J38" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K38" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="L38" s="12" t="s">
         <v>5</v>
@@ -2777,8 +2774,8 @@
       <c r="M38" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N38" s="22">
-        <v>28564569</v>
+      <c r="N38" s="20">
+        <v>29274866</v>
       </c>
       <c r="O38" s="19"/>
       <c r="P38" s="17"/>
@@ -2791,7 +2788,7 @@
         <v>4</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D39" s="12" t="s">
         <v>5</v>
@@ -2809,7 +2806,7 @@
         <v>2</v>
       </c>
       <c r="I39" s="21" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J39" s="12" t="s">
         <v>5</v>
@@ -2831,13 +2828,13 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="12" t="s">
-        <v>25</v>
+      <c r="C40" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="D40" s="12" t="s">
         <v>5</v>
@@ -2855,7 +2852,7 @@
         <v>2</v>
       </c>
       <c r="I40" s="21" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="J40" s="12" t="s">
         <v>5</v>
@@ -2869,8 +2866,8 @@
       <c r="M40" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N40" s="20">
-        <v>29274866</v>
+      <c r="N40" s="22">
+        <v>27353271</v>
       </c>
       <c r="O40" s="19"/>
       <c r="P40" s="17"/>
@@ -2882,8 +2879,8 @@
       <c r="B41" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C41" s="13" t="s">
-        <v>44</v>
+      <c r="C41" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="D41" s="12" t="s">
         <v>5</v>
@@ -2900,8 +2897,8 @@
       <c r="H41" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I41" s="21" t="s">
-        <v>45</v>
+      <c r="I41" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="J41" s="12" t="s">
         <v>5</v>
@@ -2915,15 +2912,15 @@
       <c r="M41" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N41" s="22">
-        <v>27353271</v>
-      </c>
-      <c r="O41" s="19"/>
+      <c r="N41" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="O41" s="16"/>
       <c r="P41" s="17"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>4</v>
@@ -2946,8 +2943,8 @@
       <c r="H42" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I42" s="14" t="s">
-        <v>101</v>
+      <c r="I42" s="21" t="s">
+        <v>18</v>
       </c>
       <c r="J42" s="12" t="s">
         <v>5</v>
@@ -2961,15 +2958,15 @@
       <c r="M42" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N42" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="O42" s="16"/>
+      <c r="N42" s="20">
+        <v>29274866</v>
+      </c>
+      <c r="O42" s="19"/>
       <c r="P42" s="17"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B43" s="11" t="s">
         <v>4</v>
@@ -3015,12 +3012,12 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C44" s="13" t="s">
         <v>10</v>
       </c>
       <c r="D44" s="12" t="s">
@@ -3039,7 +3036,7 @@
         <v>2</v>
       </c>
       <c r="I44" s="21" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="J44" s="12" t="s">
         <v>5</v>
@@ -3053,15 +3050,15 @@
       <c r="M44" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N44" s="20">
-        <v>29274866</v>
+      <c r="N44" s="22">
+        <v>27353271</v>
       </c>
       <c r="O44" s="19"/>
       <c r="P44" s="17"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A45" s="12" t="s">
-        <v>1</v>
+      <c r="A45" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="B45" s="11" t="s">
         <v>4</v>
@@ -3085,7 +3082,7 @@
         <v>2</v>
       </c>
       <c r="I45" s="21" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="J45" s="12" t="s">
         <v>5</v>
@@ -3107,7 +3104,7 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="13" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B46" s="11" t="s">
         <v>4</v>
@@ -3115,29 +3112,29 @@
       <c r="C46" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D46" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E46" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F46" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G46" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H46" s="12" t="s">
-        <v>2</v>
+      <c r="D46" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G46" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H46" s="13" t="s">
+        <v>0</v>
       </c>
       <c r="I46" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="J46" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="K46" s="12" t="s">
-        <v>5</v>
+        <v>5</v>
+      </c>
+      <c r="J46" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="K46" s="13" t="s">
+        <v>110</v>
       </c>
       <c r="L46" s="12" t="s">
         <v>5</v>
@@ -3146,14 +3143,14 @@
         <v>5</v>
       </c>
       <c r="N46" s="22">
-        <v>27353271</v>
+        <v>28564569</v>
       </c>
       <c r="O46" s="19"/>
       <c r="P46" s="17"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="13" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="B47" s="11" t="s">
         <v>4</v>
@@ -3162,10 +3159,10 @@
         <v>10</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F47" s="13" t="s">
         <v>5</v>
@@ -3180,10 +3177,10 @@
         <v>5</v>
       </c>
       <c r="J47" s="13" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="K47" s="13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="L47" s="12" t="s">
         <v>5</v>
@@ -3191,15 +3188,15 @@
       <c r="M47" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N47" s="22">
-        <v>28564569</v>
+      <c r="N47" s="20">
+        <v>28498551</v>
       </c>
       <c r="O47" s="19"/>
       <c r="P47" s="17"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B48" s="11" t="s">
         <v>4</v>
@@ -3208,13 +3205,13 @@
         <v>10</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E48" s="13" t="s">
         <v>134</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G48" s="13" t="s">
         <v>7</v>
@@ -3226,11 +3223,11 @@
         <v>5</v>
       </c>
       <c r="J48" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="K48" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="K48" s="13" t="s">
-        <v>113</v>
-      </c>
       <c r="L48" s="12" t="s">
         <v>5</v>
       </c>
@@ -3238,44 +3235,44 @@
         <v>5</v>
       </c>
       <c r="N48" s="20">
-        <v>28498551</v>
+        <v>26569658</v>
       </c>
       <c r="O48" s="19"/>
       <c r="P48" s="17"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A49" s="13" t="s">
+      <c r="A49" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B49" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C49" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="E49" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="F49" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G49" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H49" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="I49" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="J49" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="K49" s="13" t="s">
-        <v>113</v>
+      <c r="C49" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F49" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H49" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I49" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J49" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K49" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="L49" s="12" t="s">
         <v>5</v>
@@ -3284,44 +3281,44 @@
         <v>5</v>
       </c>
       <c r="N49" s="20">
-        <v>26569658</v>
+        <v>29274866</v>
       </c>
       <c r="O49" s="19"/>
       <c r="P49" s="17"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A50" s="12" t="s">
+      <c r="A50" s="13" t="s">
         <v>17</v>
       </c>
       <c r="B50" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C50" s="12" t="s">
+      <c r="C50" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D50" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F50" s="12" t="s">
+      <c r="D50" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E50" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="F50" s="13" t="s">
         <v>5</v>
       </c>
       <c r="G50" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H50" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="I50" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="J50" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="K50" s="12" t="s">
-        <v>5</v>
+      <c r="H50" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="I50" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="J50" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="K50" s="23" t="s">
+        <v>112</v>
       </c>
       <c r="L50" s="12" t="s">
         <v>5</v>
@@ -3330,14 +3327,14 @@
         <v>5</v>
       </c>
       <c r="N50" s="20">
-        <v>29274866</v>
+        <v>29221887</v>
       </c>
       <c r="O50" s="19"/>
       <c r="P50" s="17"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="13" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B51" s="11" t="s">
         <v>4</v>
@@ -3346,28 +3343,28 @@
         <v>31</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E51" s="13" t="s">
         <v>134</v>
       </c>
       <c r="F51" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="G51" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="G51" s="13" t="s">
         <v>7</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="I51" s="21" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="J51" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="K51" s="23" t="s">
-        <v>113</v>
+        <v>107</v>
+      </c>
+      <c r="K51" s="13" t="s">
+        <v>109</v>
       </c>
       <c r="L51" s="12" t="s">
         <v>5</v>
@@ -3375,45 +3372,45 @@
       <c r="M51" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N51" s="20">
-        <v>29221887</v>
+      <c r="N51" s="22">
+        <v>28564569</v>
       </c>
       <c r="O51" s="19"/>
       <c r="P51" s="17"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A52" s="13" t="s">
+      <c r="A52" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B52" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C52" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D52" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="E52" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="F52" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="G52" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H52" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="I52" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="J52" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="K52" s="13" t="s">
-        <v>110</v>
+      <c r="C52" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F52" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G52" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H52" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I52" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J52" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K52" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="L52" s="12" t="s">
         <v>5</v>
@@ -3421,15 +3418,15 @@
       <c r="M52" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N52" s="22">
-        <v>28564569</v>
+      <c r="N52" s="20">
+        <v>29274866</v>
       </c>
       <c r="O52" s="19"/>
       <c r="P52" s="17"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="12" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B53" s="11" t="s">
         <v>4</v>
@@ -3452,8 +3449,8 @@
       <c r="H53" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I53" s="14" t="s">
-        <v>14</v>
+      <c r="I53" s="21" t="s">
+        <v>18</v>
       </c>
       <c r="J53" s="12" t="s">
         <v>5</v>
@@ -3475,7 +3472,7 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" s="12" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B54" s="11" t="s">
         <v>4</v>
@@ -3499,7 +3496,7 @@
         <v>2</v>
       </c>
       <c r="I54" s="21" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J54" s="12" t="s">
         <v>5</v>
@@ -3521,7 +3518,7 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" s="12" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B55" s="11" t="s">
         <v>4</v>
@@ -3567,12 +3564,12 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" s="12" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="B56" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C56" s="12" t="s">
+      <c r="C56" s="13" t="s">
         <v>30</v>
       </c>
       <c r="D56" s="12" t="s">
@@ -3591,7 +3588,7 @@
         <v>2</v>
       </c>
       <c r="I56" s="21" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="J56" s="12" t="s">
         <v>5</v>
@@ -3605,15 +3602,15 @@
       <c r="M56" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N56" s="20">
-        <v>29274866</v>
+      <c r="N56" s="22">
+        <v>27353271</v>
       </c>
       <c r="O56" s="19"/>
       <c r="P56" s="17"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A57" s="12" t="s">
-        <v>1</v>
+      <c r="A57" s="13" t="s">
+        <v>17</v>
       </c>
       <c r="B57" s="11" t="s">
         <v>4</v>
@@ -3637,7 +3634,7 @@
         <v>2</v>
       </c>
       <c r="I57" s="21" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J57" s="12" t="s">
         <v>5</v>
@@ -3659,7 +3656,7 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" s="13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B58" s="11" t="s">
         <v>4</v>
@@ -3683,7 +3680,7 @@
         <v>2</v>
       </c>
       <c r="I58" s="21" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="J58" s="12" t="s">
         <v>5</v>
@@ -3705,7 +3702,7 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B59" s="11" t="s">
         <v>4</v>
@@ -3713,29 +3710,29 @@
       <c r="C59" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D59" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E59" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F59" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G59" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H59" s="12" t="s">
-        <v>2</v>
+      <c r="D59" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E59" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="F59" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G59" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H59" s="13" t="s">
+        <v>0</v>
       </c>
       <c r="I59" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="J59" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="K59" s="12" t="s">
-        <v>5</v>
+        <v>5</v>
+      </c>
+      <c r="J59" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="K59" s="13" t="s">
+        <v>112</v>
       </c>
       <c r="L59" s="12" t="s">
         <v>5</v>
@@ -3743,15 +3740,15 @@
       <c r="M59" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N59" s="22">
-        <v>27353271</v>
+      <c r="N59" s="20">
+        <v>26569658</v>
       </c>
       <c r="O59" s="19"/>
       <c r="P59" s="17"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" s="13" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B60" s="11" t="s">
         <v>4</v>
@@ -3759,29 +3756,29 @@
       <c r="C60" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D60" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="E60" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="F60" s="13" t="s">
-        <v>6</v>
+      <c r="D60" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E60" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="G60" s="13" t="s">
         <v>7</v>
       </c>
       <c r="H60" s="13" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I60" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="J60" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="K60" s="13" t="s">
-        <v>113</v>
+      <c r="J60" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K60" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="L60" s="12" t="s">
         <v>5</v>
@@ -3789,21 +3786,21 @@
       <c r="M60" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N60" s="20">
-        <v>26569658</v>
+      <c r="N60" s="22">
+        <v>29454794</v>
       </c>
       <c r="O60" s="19"/>
       <c r="P60" s="17"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A61" s="13" t="s">
-        <v>27</v>
+      <c r="A61" s="12" t="s">
+        <v>1</v>
       </c>
       <c r="B61" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C61" s="13" t="s">
-        <v>30</v>
+      <c r="C61" s="12" t="s">
+        <v>121</v>
       </c>
       <c r="D61" s="12" t="s">
         <v>5</v>
@@ -3814,14 +3811,14 @@
       <c r="F61" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G61" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H61" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="I61" s="21" t="s">
-        <v>116</v>
+      <c r="G61" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H61" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I61" s="14" t="s">
+        <v>14</v>
       </c>
       <c r="J61" s="12" t="s">
         <v>5</v>
@@ -3835,21 +3832,21 @@
       <c r="M61" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N61" s="22">
-        <v>29454794</v>
+      <c r="N61" s="20">
+        <v>29274866</v>
       </c>
       <c r="O61" s="19"/>
       <c r="P61" s="17"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" s="12" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B62" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D62" s="12" t="s">
         <v>5</v>
@@ -3889,13 +3886,13 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" s="12" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B63" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C63" s="12" t="s">
-        <v>122</v>
+      <c r="C63" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="D63" s="12" t="s">
         <v>5</v>
@@ -3912,8 +3909,8 @@
       <c r="H63" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I63" s="14" t="s">
-        <v>14</v>
+      <c r="I63" s="21" t="s">
+        <v>47</v>
       </c>
       <c r="J63" s="12" t="s">
         <v>5</v>
@@ -3927,8 +3924,8 @@
       <c r="M63" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N63" s="20">
-        <v>29274866</v>
+      <c r="N63" s="22">
+        <v>27353271</v>
       </c>
       <c r="O63" s="19"/>
       <c r="P63" s="17"/>
@@ -3941,7 +3938,7 @@
         <v>4</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D64" s="12" t="s">
         <v>5</v>
@@ -3959,7 +3956,7 @@
         <v>2</v>
       </c>
       <c r="I64" s="21" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="J64" s="12" t="s">
         <v>5</v>
@@ -3980,38 +3977,38 @@
       <c r="P64" s="17"/>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A65" s="12" t="s">
-        <v>32</v>
+      <c r="A65" s="13" t="s">
+        <v>1</v>
       </c>
       <c r="B65" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C65" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="D65" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E65" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F65" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G65" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H65" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="I65" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="J65" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="K65" s="12" t="s">
-        <v>5</v>
+      <c r="C65" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="D65" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E65" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="F65" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G65" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H65" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="I65" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="J65" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="K65" s="13" t="s">
+        <v>110</v>
       </c>
       <c r="L65" s="12" t="s">
         <v>5</v>
@@ -4019,21 +4016,21 @@
       <c r="M65" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N65" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="O65" s="16"/>
+      <c r="N65" s="22">
+        <v>28564569</v>
+      </c>
+      <c r="O65" s="19"/>
       <c r="P65" s="17"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" s="12" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="B66" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C66" s="13" t="s">
-        <v>48</v>
+      <c r="C66" s="12" t="s">
+        <v>102</v>
       </c>
       <c r="D66" s="12" t="s">
         <v>5</v>
@@ -4050,8 +4047,8 @@
       <c r="H66" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I66" s="21" t="s">
-        <v>49</v>
+      <c r="I66" s="14" t="s">
+        <v>60</v>
       </c>
       <c r="J66" s="12" t="s">
         <v>5</v>
@@ -4065,45 +4062,45 @@
       <c r="M66" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N66" s="22">
-        <v>27353271</v>
-      </c>
-      <c r="O66" s="19"/>
+      <c r="N66" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="O66" s="16"/>
       <c r="P66" s="17"/>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A67" s="13" t="s">
-        <v>1</v>
+      <c r="A67" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="B67" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C67" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="D67" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="E67" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="F67" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G67" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H67" s="13" t="s">
-        <v>0</v>
+      <c r="C67" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E67" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F67" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H67" s="12" t="s">
+        <v>2</v>
       </c>
       <c r="I67" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="J67" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="K67" s="13" t="s">
-        <v>111</v>
+        <v>14</v>
+      </c>
+      <c r="J67" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K67" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="L67" s="12" t="s">
         <v>5</v>
@@ -4111,21 +4108,21 @@
       <c r="M67" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N67" s="22">
-        <v>28564569</v>
+      <c r="N67" s="20">
+        <v>29274866</v>
       </c>
       <c r="O67" s="19"/>
       <c r="P67" s="17"/>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68" s="12" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="B68" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="D68" s="12" t="s">
         <v>5</v>
@@ -4142,8 +4139,8 @@
       <c r="H68" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I68" s="14" t="s">
-        <v>60</v>
+      <c r="I68" s="14">
+        <v>10.9</v>
       </c>
       <c r="J68" s="12" t="s">
         <v>5</v>
@@ -4158,20 +4155,20 @@
         <v>5</v>
       </c>
       <c r="N68" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O68" s="16"/>
       <c r="P68" s="17"/>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69" s="12" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="B69" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D69" s="12" t="s">
         <v>5</v>
@@ -4216,7 +4213,7 @@
       <c r="B70" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C70" s="12" t="s">
+      <c r="C70" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D70" s="12" t="s">
@@ -4234,8 +4231,8 @@
       <c r="H70" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I70" s="14">
-        <v>10.9</v>
+      <c r="I70" s="21" t="s">
+        <v>50</v>
       </c>
       <c r="J70" s="12" t="s">
         <v>5</v>
@@ -4249,10 +4246,10 @@
       <c r="M70" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N70" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="O70" s="16"/>
+      <c r="N70" s="22">
+        <v>27353271</v>
+      </c>
+      <c r="O70" s="19"/>
       <c r="P70" s="17"/>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.2">
@@ -4262,8 +4259,8 @@
       <c r="B71" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C71" s="12" t="s">
-        <v>13</v>
+      <c r="C71" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="D71" s="12" t="s">
         <v>5</v>
@@ -4281,7 +4278,7 @@
         <v>2</v>
       </c>
       <c r="I71" s="21" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="J71" s="12" t="s">
         <v>5</v>
@@ -4295,8 +4292,8 @@
       <c r="M71" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N71" s="20">
-        <v>29274866</v>
+      <c r="N71" s="22">
+        <v>27353271</v>
       </c>
       <c r="O71" s="19"/>
       <c r="P71" s="17"/>
@@ -4309,7 +4306,7 @@
         <v>4</v>
       </c>
       <c r="C72" s="13" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D72" s="12" t="s">
         <v>5</v>
@@ -4326,8 +4323,8 @@
       <c r="H72" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I72" s="21" t="s">
-        <v>50</v>
+      <c r="I72" s="14">
+        <v>609.1</v>
       </c>
       <c r="J72" s="12" t="s">
         <v>5</v>
@@ -4341,21 +4338,21 @@
       <c r="M72" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N72" s="22">
-        <v>27353271</v>
-      </c>
-      <c r="O72" s="19"/>
+      <c r="N72" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="O72" s="16"/>
       <c r="P72" s="17"/>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73" s="12" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B73" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C73" s="13" t="s">
-        <v>59</v>
+      <c r="C73" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="D73" s="12" t="s">
         <v>5</v>
@@ -4372,8 +4369,8 @@
       <c r="H73" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I73" s="21" t="s">
-        <v>60</v>
+      <c r="I73" s="14">
+        <v>246.2</v>
       </c>
       <c r="J73" s="12" t="s">
         <v>5</v>
@@ -4387,8 +4384,8 @@
       <c r="M73" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N73" s="22">
-        <v>27353271</v>
+      <c r="N73" s="15" t="s">
+        <v>132</v>
       </c>
       <c r="O73" s="19"/>
       <c r="P73" s="17"/>
@@ -4400,7 +4397,7 @@
       <c r="B74" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C74" s="13" t="s">
+      <c r="C74" s="12" t="s">
         <v>6</v>
       </c>
       <c r="D74" s="12" t="s">
@@ -4418,8 +4415,8 @@
       <c r="H74" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I74" s="14">
-        <v>609.1</v>
+      <c r="I74" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="J74" s="12" t="s">
         <v>5</v>
@@ -4433,15 +4430,15 @@
       <c r="M74" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N74" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="O74" s="16"/>
+      <c r="N74" s="20">
+        <v>29274866</v>
+      </c>
+      <c r="O74" s="19"/>
       <c r="P74" s="17"/>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A75" s="12" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B75" s="11" t="s">
         <v>4</v>
@@ -4464,8 +4461,8 @@
       <c r="H75" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I75" s="14">
-        <v>246.2</v>
+      <c r="I75" s="21" t="s">
+        <v>14</v>
       </c>
       <c r="J75" s="12" t="s">
         <v>5</v>
@@ -4479,15 +4476,15 @@
       <c r="M75" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N75" s="15" t="s">
-        <v>133</v>
+      <c r="N75" s="20">
+        <v>29274866</v>
       </c>
       <c r="O75" s="19"/>
       <c r="P75" s="17"/>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A76" s="12" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="B76" s="11" t="s">
         <v>4</v>
@@ -4510,8 +4507,8 @@
       <c r="H76" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I76" s="14" t="s">
-        <v>12</v>
+      <c r="I76" s="21" t="s">
+        <v>14</v>
       </c>
       <c r="J76" s="12" t="s">
         <v>5</v>
@@ -4533,7 +4530,7 @@
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A77" s="12" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B77" s="11" t="s">
         <v>4</v>
@@ -4557,7 +4554,7 @@
         <v>2</v>
       </c>
       <c r="I77" s="21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J77" s="12" t="s">
         <v>5</v>
@@ -4579,12 +4576,12 @@
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A78" s="12" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="B78" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C78" s="12" t="s">
+      <c r="C78" s="13" t="s">
         <v>6</v>
       </c>
       <c r="D78" s="12" t="s">
@@ -4603,7 +4600,7 @@
         <v>2</v>
       </c>
       <c r="I78" s="21" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="J78" s="12" t="s">
         <v>5</v>
@@ -4617,20 +4614,20 @@
       <c r="M78" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N78" s="20">
-        <v>29274866</v>
+      <c r="N78" s="22">
+        <v>27353271</v>
       </c>
       <c r="O78" s="19"/>
       <c r="P78" s="17"/>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A79" s="12" t="s">
-        <v>11</v>
+      <c r="A79" s="13" t="s">
+        <v>17</v>
       </c>
       <c r="B79" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C79" s="12" t="s">
+      <c r="C79" s="13" t="s">
         <v>6</v>
       </c>
       <c r="D79" s="12" t="s">
@@ -4649,7 +4646,7 @@
         <v>2</v>
       </c>
       <c r="I79" s="21" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="J79" s="12" t="s">
         <v>5</v>
@@ -4663,15 +4660,15 @@
       <c r="M79" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N79" s="20">
-        <v>29274866</v>
+      <c r="N79" s="22">
+        <v>27353271</v>
       </c>
       <c r="O79" s="19"/>
       <c r="P79" s="17"/>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A80" s="12" t="s">
-        <v>1</v>
+      <c r="A80" s="13" t="s">
+        <v>19</v>
       </c>
       <c r="B80" s="11" t="s">
         <v>4</v>
@@ -4695,7 +4692,7 @@
         <v>2</v>
       </c>
       <c r="I80" s="21" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="J80" s="12" t="s">
         <v>5</v>
@@ -4717,7 +4714,7 @@
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A81" s="13" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B81" s="11" t="s">
         <v>4</v>
@@ -4741,7 +4738,7 @@
         <v>2</v>
       </c>
       <c r="I81" s="21" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="J81" s="12" t="s">
         <v>5</v>
@@ -4763,7 +4760,7 @@
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A82" s="13" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="B82" s="11" t="s">
         <v>4</v>
@@ -4787,7 +4784,7 @@
         <v>2</v>
       </c>
       <c r="I82" s="21" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="J82" s="12" t="s">
         <v>5</v>
@@ -4809,7 +4806,7 @@
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A83" s="13" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B83" s="11" t="s">
         <v>4</v>
@@ -4817,29 +4814,29 @@
       <c r="C83" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D83" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E83" s="12" t="s">
-        <v>5</v>
+      <c r="D83" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E83" s="13" t="s">
+        <v>134</v>
       </c>
       <c r="F83" s="12" t="s">
-        <v>5</v>
+        <v>135</v>
       </c>
       <c r="G83" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H83" s="12" t="s">
-        <v>2</v>
+      <c r="H83" s="13" t="s">
+        <v>82</v>
       </c>
       <c r="I83" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="J83" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="K83" s="12" t="s">
-        <v>5</v>
+        <v>83</v>
+      </c>
+      <c r="J83" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="K83" s="23" t="s">
+        <v>112</v>
       </c>
       <c r="L83" s="12" t="s">
         <v>5</v>
@@ -4847,15 +4844,15 @@
       <c r="M83" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N83" s="22">
-        <v>27353271</v>
-      </c>
-      <c r="O83" s="19"/>
+      <c r="N83" s="20">
+        <v>29221887</v>
+      </c>
+      <c r="O83" s="24"/>
       <c r="P83" s="17"/>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A84" s="13" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="B84" s="11" t="s">
         <v>4</v>
@@ -4863,45 +4860,45 @@
       <c r="C84" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D84" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E84" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F84" s="12" t="s">
-        <v>5</v>
+      <c r="D84" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E84" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="F84" s="13" t="s">
+        <v>65</v>
       </c>
       <c r="G84" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H84" s="12" t="s">
-        <v>2</v>
+      <c r="H84" s="13" t="s">
+        <v>82</v>
       </c>
       <c r="I84" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="J84" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="K84" s="12" t="s">
-        <v>5</v>
+        <v>86</v>
+      </c>
+      <c r="J84" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="K84" s="23" t="s">
+        <v>112</v>
       </c>
       <c r="L84" s="12" t="s">
         <v>5</v>
       </c>
       <c r="M84" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="N84" s="22">
-        <v>27353271</v>
-      </c>
-      <c r="O84" s="19"/>
+        <v>136</v>
+      </c>
+      <c r="N84" s="20">
+        <v>29221887</v>
+      </c>
+      <c r="O84" s="24"/>
       <c r="P84" s="17"/>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A85" s="13" t="s">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="B85" s="11" t="s">
         <v>4</v>
@@ -4910,13 +4907,13 @@
         <v>6</v>
       </c>
       <c r="D85" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E85" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="E85" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="F85" s="12" t="s">
-        <v>136</v>
+      <c r="F85" s="13" t="s">
+        <v>65</v>
       </c>
       <c r="G85" s="12" t="s">
         <v>7</v>
@@ -4925,19 +4922,19 @@
         <v>82</v>
       </c>
       <c r="I85" s="21" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J85" s="13" t="s">
         <v>80</v>
       </c>
       <c r="K85" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L85" s="12" t="s">
         <v>5</v>
       </c>
       <c r="M85" s="12" t="s">
-        <v>5</v>
+        <v>136</v>
       </c>
       <c r="N85" s="20">
         <v>29221887</v>
@@ -4947,7 +4944,7 @@
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A86" s="13" t="s">
-        <v>120</v>
+        <v>11</v>
       </c>
       <c r="B86" s="11" t="s">
         <v>4</v>
@@ -4959,10 +4956,10 @@
         <v>134</v>
       </c>
       <c r="E86" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="F86" s="13" t="s">
         <v>135</v>
-      </c>
-      <c r="F86" s="13" t="s">
-        <v>65</v>
       </c>
       <c r="G86" s="12" t="s">
         <v>7</v>
@@ -4971,19 +4968,19 @@
         <v>82</v>
       </c>
       <c r="I86" s="21" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J86" s="13" t="s">
         <v>80</v>
       </c>
       <c r="K86" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L86" s="12" t="s">
         <v>5</v>
       </c>
       <c r="M86" s="12" t="s">
-        <v>137</v>
+        <v>5</v>
       </c>
       <c r="N86" s="20">
         <v>29221887</v>
@@ -4993,7 +4990,7 @@
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A87" s="13" t="s">
-        <v>121</v>
+        <v>11</v>
       </c>
       <c r="B87" s="11" t="s">
         <v>4</v>
@@ -5002,13 +4999,13 @@
         <v>6</v>
       </c>
       <c r="D87" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E87" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="E87" s="13" t="s">
-        <v>135</v>
-      </c>
       <c r="F87" s="13" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="G87" s="12" t="s">
         <v>7</v>
@@ -5017,19 +5014,19 @@
         <v>82</v>
       </c>
       <c r="I87" s="21" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="J87" s="13" t="s">
         <v>80</v>
       </c>
       <c r="K87" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L87" s="12" t="s">
         <v>5</v>
       </c>
       <c r="M87" s="12" t="s">
-        <v>137</v>
+        <v>5</v>
       </c>
       <c r="N87" s="20">
         <v>29221887</v>
@@ -5048,13 +5045,13 @@
         <v>6</v>
       </c>
       <c r="D88" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E88" s="13" t="s">
         <v>134</v>
       </c>
       <c r="F88" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G88" s="12" t="s">
         <v>7</v>
@@ -5063,13 +5060,13 @@
         <v>82</v>
       </c>
       <c r="I88" s="21" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="J88" s="13" t="s">
         <v>80</v>
       </c>
       <c r="K88" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L88" s="12" t="s">
         <v>5</v>
@@ -5097,25 +5094,25 @@
         <v>134</v>
       </c>
       <c r="E89" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F89" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G89" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G89" s="13" t="s">
         <v>7</v>
       </c>
       <c r="H89" s="13" t="s">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="I89" s="21" t="s">
-        <v>89</v>
+        <v>5</v>
       </c>
       <c r="J89" s="13" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="K89" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L89" s="12" t="s">
         <v>5</v>
@@ -5123,8 +5120,8 @@
       <c r="M89" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N89" s="20">
-        <v>29221887</v>
+      <c r="N89" s="22">
+        <v>26575258</v>
       </c>
       <c r="O89" s="24"/>
       <c r="P89" s="17"/>
@@ -5140,28 +5137,28 @@
         <v>6</v>
       </c>
       <c r="D90" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E90" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="E90" s="13" t="s">
+      <c r="F90" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="F90" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="G90" s="12" t="s">
+      <c r="G90" s="13" t="s">
         <v>7</v>
       </c>
       <c r="H90" s="13" t="s">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="I90" s="21" t="s">
-        <v>90</v>
+        <v>5</v>
       </c>
       <c r="J90" s="13" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="K90" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L90" s="12" t="s">
         <v>5</v>
@@ -5169,15 +5166,15 @@
       <c r="M90" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N90" s="20">
-        <v>29221887</v>
+      <c r="N90" s="22">
+        <v>26575258</v>
       </c>
       <c r="O90" s="24"/>
       <c r="P90" s="17"/>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A91" s="13" t="s">
-        <v>11</v>
+      <c r="A91" s="13">
+        <v>3</v>
       </c>
       <c r="B91" s="11" t="s">
         <v>4</v>
@@ -5186,13 +5183,13 @@
         <v>6</v>
       </c>
       <c r="D91" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E91" s="13" t="s">
         <v>134</v>
       </c>
       <c r="F91" s="13" t="s">
-        <v>5</v>
+        <v>135</v>
       </c>
       <c r="G91" s="13" t="s">
         <v>7</v>
@@ -5207,7 +5204,7 @@
         <v>93</v>
       </c>
       <c r="K91" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L91" s="12" t="s">
         <v>5</v>
@@ -5232,13 +5229,13 @@
         <v>6</v>
       </c>
       <c r="D92" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E92" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="E92" s="13" t="s">
-        <v>135</v>
-      </c>
       <c r="F92" s="13" t="s">
-        <v>136</v>
+        <v>15</v>
       </c>
       <c r="G92" s="13" t="s">
         <v>7</v>
@@ -5253,7 +5250,7 @@
         <v>93</v>
       </c>
       <c r="K92" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L92" s="12" t="s">
         <v>5</v>
@@ -5268,8 +5265,8 @@
       <c r="P92" s="17"/>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A93" s="13">
-        <v>3</v>
+      <c r="A93" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="B93" s="11" t="s">
         <v>4</v>
@@ -5281,10 +5278,10 @@
         <v>134</v>
       </c>
       <c r="E93" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>136</v>
+        <v>5</v>
       </c>
       <c r="G93" s="13" t="s">
         <v>7</v>
@@ -5296,10 +5293,10 @@
         <v>5</v>
       </c>
       <c r="J93" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="K93" s="23" t="s">
-        <v>113</v>
+        <v>107</v>
+      </c>
+      <c r="K93" s="13" t="s">
+        <v>109</v>
       </c>
       <c r="L93" s="12" t="s">
         <v>5</v>
@@ -5308,14 +5305,14 @@
         <v>5</v>
       </c>
       <c r="N93" s="22">
-        <v>26575258</v>
+        <v>28564569</v>
       </c>
       <c r="O93" s="24"/>
       <c r="P93" s="17"/>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A94" s="13" t="s">
-        <v>11</v>
+        <v>103</v>
       </c>
       <c r="B94" s="11" t="s">
         <v>4</v>
@@ -5324,13 +5321,13 @@
         <v>6</v>
       </c>
       <c r="D94" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E94" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="E94" s="13" t="s">
-        <v>135</v>
-      </c>
       <c r="F94" s="13" t="s">
-        <v>15</v>
+        <v>137</v>
       </c>
       <c r="G94" s="13" t="s">
         <v>7</v>
@@ -5342,10 +5339,10 @@
         <v>5</v>
       </c>
       <c r="J94" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="K94" s="23" t="s">
-        <v>113</v>
+        <v>107</v>
+      </c>
+      <c r="K94" s="13" t="s">
+        <v>109</v>
       </c>
       <c r="L94" s="12" t="s">
         <v>5</v>
@@ -5354,14 +5351,14 @@
         <v>5</v>
       </c>
       <c r="N94" s="22">
-        <v>26575258</v>
+        <v>28564569</v>
       </c>
       <c r="O94" s="24"/>
       <c r="P94" s="17"/>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="13" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B95" s="11" t="s">
         <v>4</v>
@@ -5370,13 +5367,13 @@
         <v>6</v>
       </c>
       <c r="D95" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E95" s="13" t="s">
         <v>134</v>
       </c>
       <c r="F95" s="13" t="s">
-        <v>5</v>
+        <v>135</v>
       </c>
       <c r="G95" s="13" t="s">
         <v>7</v>
@@ -5407,7 +5404,7 @@
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A96" s="13" t="s">
-        <v>104</v>
+        <v>11</v>
       </c>
       <c r="B96" s="11" t="s">
         <v>4</v>
@@ -5416,13 +5413,13 @@
         <v>6</v>
       </c>
       <c r="D96" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E96" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="E96" s="13" t="s">
+      <c r="F96" s="13" t="s">
         <v>135</v>
-      </c>
-      <c r="F96" s="13" t="s">
-        <v>138</v>
       </c>
       <c r="G96" s="13" t="s">
         <v>7</v>
@@ -5451,9 +5448,9 @@
       <c r="O96" s="24"/>
       <c r="P96" s="17"/>
     </row>
-    <row r="97" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A97" s="13" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B97" s="11" t="s">
         <v>4</v>
@@ -5462,13 +5459,13 @@
         <v>6</v>
       </c>
       <c r="D97" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E97" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="E97" s="13" t="s">
-        <v>135</v>
-      </c>
       <c r="F97" s="13" t="s">
-        <v>136</v>
+        <v>15</v>
       </c>
       <c r="G97" s="13" t="s">
         <v>7</v>
@@ -5480,10 +5477,10 @@
         <v>5</v>
       </c>
       <c r="J97" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K97" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L97" s="12" t="s">
         <v>5</v>
@@ -5499,7 +5496,7 @@
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A98" s="13" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B98" s="11" t="s">
         <v>4</v>
@@ -5508,13 +5505,13 @@
         <v>6</v>
       </c>
       <c r="D98" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E98" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="E98" s="13" t="s">
-        <v>135</v>
-      </c>
       <c r="F98" s="13" t="s">
-        <v>136</v>
+        <v>106</v>
       </c>
       <c r="G98" s="13" t="s">
         <v>7</v>
@@ -5526,16 +5523,16 @@
         <v>5</v>
       </c>
       <c r="J98" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K98" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L98" s="12" t="s">
         <v>5</v>
       </c>
       <c r="M98" s="12" t="s">
-        <v>5</v>
+        <v>139</v>
       </c>
       <c r="N98" s="22">
         <v>28564569</v>
@@ -5545,7 +5542,7 @@
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A99" s="13" t="s">
-        <v>11</v>
+        <v>117</v>
       </c>
       <c r="B99" s="11" t="s">
         <v>4</v>
@@ -5554,13 +5551,13 @@
         <v>6</v>
       </c>
       <c r="D99" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E99" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="E99" s="13" t="s">
-        <v>135</v>
-      </c>
       <c r="F99" s="13" t="s">
-        <v>15</v>
+        <v>106</v>
       </c>
       <c r="G99" s="13" t="s">
         <v>7</v>
@@ -5572,16 +5569,16 @@
         <v>5</v>
       </c>
       <c r="J99" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K99" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L99" s="12" t="s">
         <v>5</v>
       </c>
       <c r="M99" s="12" t="s">
-        <v>5</v>
+        <v>139</v>
       </c>
       <c r="N99" s="22">
         <v>28564569</v>
@@ -5591,7 +5588,7 @@
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A100" s="13" t="s">
-        <v>19</v>
+        <v>118</v>
       </c>
       <c r="B100" s="11" t="s">
         <v>4</v>
@@ -5600,13 +5597,13 @@
         <v>6</v>
       </c>
       <c r="D100" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E100" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="E100" s="13" t="s">
-        <v>135</v>
-      </c>
       <c r="F100" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G100" s="13" t="s">
         <v>7</v>
@@ -5618,16 +5615,16 @@
         <v>5</v>
       </c>
       <c r="J100" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K100" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L100" s="12" t="s">
         <v>5</v>
       </c>
       <c r="M100" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N100" s="22">
         <v>28564569</v>
@@ -5637,7 +5634,7 @@
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A101" s="13" t="s">
-        <v>118</v>
+        <v>11</v>
       </c>
       <c r="B101" s="11" t="s">
         <v>4</v>
@@ -5649,10 +5646,10 @@
         <v>134</v>
       </c>
       <c r="E101" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F101" s="13" t="s">
-        <v>107</v>
+        <v>5</v>
       </c>
       <c r="G101" s="13" t="s">
         <v>7</v>
@@ -5664,26 +5661,26 @@
         <v>5</v>
       </c>
       <c r="J101" s="13" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="K101" s="13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="L101" s="12" t="s">
         <v>5</v>
       </c>
       <c r="M101" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="N101" s="22">
-        <v>28564569</v>
+        <v>5</v>
+      </c>
+      <c r="N101" s="20">
+        <v>28498551</v>
       </c>
       <c r="O101" s="24"/>
       <c r="P101" s="17"/>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A102" s="13" t="s">
-        <v>119</v>
+        <v>11</v>
       </c>
       <c r="B102" s="11" t="s">
         <v>4</v>
@@ -5695,10 +5692,10 @@
         <v>134</v>
       </c>
       <c r="E102" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F102" s="13" t="s">
-        <v>107</v>
+        <v>5</v>
       </c>
       <c r="G102" s="13" t="s">
         <v>7</v>
@@ -5710,26 +5707,26 @@
         <v>5</v>
       </c>
       <c r="J102" s="13" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="K102" s="13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="L102" s="12" t="s">
         <v>5</v>
       </c>
       <c r="M102" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="N102" s="22">
-        <v>28564569</v>
+        <v>5</v>
+      </c>
+      <c r="N102" s="20">
+        <v>26569658</v>
       </c>
       <c r="O102" s="24"/>
       <c r="P102" s="17"/>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A103" s="13" t="s">
-        <v>11</v>
+      <c r="A103" s="13">
+        <v>3</v>
       </c>
       <c r="B103" s="11" t="s">
         <v>4</v>
@@ -5738,13 +5735,13 @@
         <v>6</v>
       </c>
       <c r="D103" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E103" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="F103" s="13" t="s">
         <v>135</v>
-      </c>
-      <c r="E103" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="F103" s="13" t="s">
-        <v>5</v>
       </c>
       <c r="G103" s="13" t="s">
         <v>7</v>
@@ -5756,11 +5753,11 @@
         <v>5</v>
       </c>
       <c r="J103" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="K103" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="K103" s="13" t="s">
-        <v>113</v>
-      </c>
       <c r="L103" s="12" t="s">
         <v>5</v>
       </c>
@@ -5768,14 +5765,14 @@
         <v>5</v>
       </c>
       <c r="N103" s="20">
-        <v>28498551</v>
+        <v>26569658</v>
       </c>
       <c r="O103" s="24"/>
       <c r="P103" s="17"/>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A104" s="13" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B104" s="11" t="s">
         <v>4</v>
@@ -5784,10 +5781,10 @@
         <v>6</v>
       </c>
       <c r="D104" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E104" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F104" s="13" t="s">
         <v>5</v>
@@ -5802,10 +5799,10 @@
         <v>5</v>
       </c>
       <c r="J104" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K104" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L104" s="12" t="s">
         <v>5</v>
@@ -5820,8 +5817,8 @@
       <c r="P104" s="17"/>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A105" s="13">
-        <v>3</v>
+      <c r="A105" s="13" t="s">
+        <v>17</v>
       </c>
       <c r="B105" s="11" t="s">
         <v>4</v>
@@ -5830,13 +5827,13 @@
         <v>6</v>
       </c>
       <c r="D105" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E105" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="E105" s="13" t="s">
-        <v>135</v>
-      </c>
       <c r="F105" s="13" t="s">
-        <v>136</v>
+        <v>10</v>
       </c>
       <c r="G105" s="13" t="s">
         <v>7</v>
@@ -5848,10 +5845,10 @@
         <v>5</v>
       </c>
       <c r="J105" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K105" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L105" s="12" t="s">
         <v>5</v>
@@ -5862,42 +5859,42 @@
       <c r="N105" s="20">
         <v>26569658</v>
       </c>
-      <c r="O105" s="24"/>
+      <c r="O105" s="19"/>
       <c r="P105" s="17"/>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A106" s="13" t="s">
-        <v>17</v>
+      <c r="A106" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="B106" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C106" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D106" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="E106" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="F106" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="G106" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H106" s="13" t="s">
-        <v>0</v>
+      <c r="C106" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D106" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E106" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F106" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G106" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H106" s="12" t="s">
+        <v>2</v>
       </c>
       <c r="I106" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="J106" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="K106" s="13" t="s">
-        <v>113</v>
+        <v>12</v>
+      </c>
+      <c r="J106" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K106" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="L106" s="12" t="s">
         <v>5</v>
@@ -5906,44 +5903,44 @@
         <v>5</v>
       </c>
       <c r="N106" s="20">
-        <v>26569658</v>
-      </c>
-      <c r="O106" s="24"/>
+        <v>29274866</v>
+      </c>
+      <c r="O106" s="19"/>
       <c r="P106" s="17"/>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A107" s="13" t="s">
-        <v>17</v>
+      <c r="A107" s="12" t="s">
+        <v>1</v>
       </c>
       <c r="B107" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C107" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D107" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="E107" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="F107" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G107" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H107" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="I107" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="J107" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="K107" s="13" t="s">
-        <v>113</v>
+      <c r="C107" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D107" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E107" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F107" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G107" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H107" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I107" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J107" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K107" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="L107" s="12" t="s">
         <v>5</v>
@@ -5952,20 +5949,20 @@
         <v>5</v>
       </c>
       <c r="N107" s="20">
-        <v>26569658</v>
+        <v>29274866</v>
       </c>
       <c r="O107" s="19"/>
       <c r="P107" s="17"/>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A108" s="12" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B108" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D108" s="12" t="s">
         <v>5</v>
@@ -5982,8 +5979,8 @@
       <c r="H108" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I108" s="21" t="s">
-        <v>12</v>
+      <c r="I108" s="14" t="s">
+        <v>18</v>
       </c>
       <c r="J108" s="12" t="s">
         <v>5</v>
@@ -6010,7 +6007,7 @@
       <c r="B109" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C109" s="12" t="s">
+      <c r="C109" s="13" t="s">
         <v>16</v>
       </c>
       <c r="D109" s="12" t="s">
@@ -6028,8 +6025,8 @@
       <c r="H109" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I109" s="14" t="s">
-        <v>14</v>
+      <c r="I109" s="21" t="s">
+        <v>52</v>
       </c>
       <c r="J109" s="12" t="s">
         <v>5</v>
@@ -6043,20 +6040,20 @@
       <c r="M109" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N109" s="20">
-        <v>29274866</v>
+      <c r="N109" s="22">
+        <v>27353271</v>
       </c>
       <c r="O109" s="19"/>
       <c r="P109" s="17"/>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A110" s="12" t="s">
+      <c r="A110" s="13" t="s">
         <v>17</v>
       </c>
       <c r="B110" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C110" s="12" t="s">
+      <c r="C110" s="13" t="s">
         <v>16</v>
       </c>
       <c r="D110" s="12" t="s">
@@ -6074,8 +6071,8 @@
       <c r="H110" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I110" s="14" t="s">
-        <v>18</v>
+      <c r="I110" s="21" t="s">
+        <v>70</v>
       </c>
       <c r="J110" s="12" t="s">
         <v>5</v>
@@ -6089,15 +6086,15 @@
       <c r="M110" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N110" s="20">
-        <v>29274866</v>
+      <c r="N110" s="22">
+        <v>27353271</v>
       </c>
       <c r="O110" s="19"/>
       <c r="P110" s="17"/>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A111" s="12" t="s">
-        <v>1</v>
+      <c r="A111" s="13" t="s">
+        <v>76</v>
       </c>
       <c r="B111" s="11" t="s">
         <v>4</v>
@@ -6121,7 +6118,7 @@
         <v>2</v>
       </c>
       <c r="I111" s="21" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="J111" s="12" t="s">
         <v>5</v>
@@ -6143,7 +6140,7 @@
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A112" s="13" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B112" s="11" t="s">
         <v>4</v>
@@ -6151,29 +6148,29 @@
       <c r="C112" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D112" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E112" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F112" s="12" t="s">
-        <v>5</v>
+      <c r="D112" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E112" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="F112" s="13" t="s">
+        <v>135</v>
       </c>
       <c r="G112" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H112" s="12" t="s">
-        <v>2</v>
+      <c r="H112" s="13" t="s">
+        <v>82</v>
       </c>
       <c r="I112" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="J112" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="K112" s="12" t="s">
-        <v>5</v>
+        <v>81</v>
+      </c>
+      <c r="J112" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="K112" s="23" t="s">
+        <v>112</v>
       </c>
       <c r="L112" s="12" t="s">
         <v>5</v>
@@ -6181,15 +6178,15 @@
       <c r="M112" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N112" s="22">
-        <v>27353271</v>
+      <c r="N112" s="20">
+        <v>29221887</v>
       </c>
       <c r="O112" s="19"/>
       <c r="P112" s="17"/>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A113" s="13" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="B113" s="11" t="s">
         <v>4</v>
@@ -6197,29 +6194,29 @@
       <c r="C113" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D113" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E113" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F113" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G113" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H113" s="12" t="s">
-        <v>2</v>
+      <c r="D113" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E113" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="F113" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G113" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H113" s="13" t="s">
+        <v>0</v>
       </c>
       <c r="I113" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="J113" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="K113" s="12" t="s">
-        <v>5</v>
+        <v>5</v>
+      </c>
+      <c r="J113" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="K113" s="13" t="s">
+        <v>109</v>
       </c>
       <c r="L113" s="12" t="s">
         <v>5</v>
@@ -6228,7 +6225,7 @@
         <v>5</v>
       </c>
       <c r="N113" s="22">
-        <v>27353271</v>
+        <v>28564569</v>
       </c>
       <c r="O113" s="19"/>
       <c r="P113" s="17"/>
@@ -6244,28 +6241,28 @@
         <v>16</v>
       </c>
       <c r="D114" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E114" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="E114" s="13" t="s">
+      <c r="F114" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="F114" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="G114" s="12" t="s">
+      <c r="G114" s="13" t="s">
         <v>7</v>
       </c>
       <c r="H114" s="13" t="s">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="I114" s="21" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="J114" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="K114" s="23" t="s">
-        <v>113</v>
+        <v>114</v>
+      </c>
+      <c r="K114" s="13" t="s">
+        <v>112</v>
       </c>
       <c r="L114" s="12" t="s">
         <v>5</v>
@@ -6274,44 +6271,44 @@
         <v>5</v>
       </c>
       <c r="N114" s="20">
-        <v>29221887</v>
+        <v>26569658</v>
       </c>
       <c r="O114" s="19"/>
       <c r="P114" s="17"/>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A115" s="13" t="s">
+      <c r="A115" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B115" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C115" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D115" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="E115" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="F115" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="G115" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H115" s="13" t="s">
-        <v>0</v>
+        <v>55</v>
+      </c>
+      <c r="D115" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E115" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F115" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G115" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H115" s="12" t="s">
+        <v>2</v>
       </c>
       <c r="I115" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="J115" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="K115" s="13" t="s">
-        <v>110</v>
+        <v>56</v>
+      </c>
+      <c r="J115" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K115" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="L115" s="12" t="s">
         <v>5</v>
@@ -6320,44 +6317,44 @@
         <v>5</v>
       </c>
       <c r="N115" s="22">
-        <v>28564569</v>
+        <v>27353271</v>
       </c>
       <c r="O115" s="19"/>
       <c r="P115" s="17"/>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A116" s="13" t="s">
+      <c r="A116" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B116" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C116" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D116" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="E116" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="F116" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="G116" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H116" s="13" t="s">
-        <v>0</v>
+        <v>57</v>
+      </c>
+      <c r="D116" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E116" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F116" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G116" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H116" s="12" t="s">
+        <v>2</v>
       </c>
       <c r="I116" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="J116" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="K116" s="13" t="s">
-        <v>113</v>
+        <v>58</v>
+      </c>
+      <c r="J116" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K116" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="L116" s="12" t="s">
         <v>5</v>
@@ -6365,8 +6362,8 @@
       <c r="M116" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N116" s="20">
-        <v>26569658</v>
+      <c r="N116" s="22">
+        <v>27353271</v>
       </c>
       <c r="O116" s="19"/>
       <c r="P116" s="17"/>
@@ -6379,7 +6376,7 @@
         <v>4</v>
       </c>
       <c r="C117" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D117" s="12" t="s">
         <v>5</v>
@@ -6397,7 +6394,7 @@
         <v>2</v>
       </c>
       <c r="I117" s="21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J117" s="12" t="s">
         <v>5</v>
@@ -6417,132 +6414,104 @@
       <c r="O117" s="19"/>
       <c r="P117" s="17"/>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A118" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B118" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C118" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D118" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E118" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F118" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G118" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H118" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="I118" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="J118" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="K118" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="L118" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="M118" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="N118" s="22">
-        <v>27353271</v>
-      </c>
-      <c r="O118" s="19"/>
-      <c r="P118" s="17"/>
-    </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A119" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B119" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C119" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="D119" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E119" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F119" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G119" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H119" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="I119" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="J119" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="K119" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="L119" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="M119" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="N119" s="22">
-        <v>27353271</v>
-      </c>
-      <c r="O119" s="19"/>
-      <c r="P119" s="17"/>
-    </row>
-    <row r="120" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="B118" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C118" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="D118" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="E118" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="F118" s="31"/>
+      <c r="G118" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="H118" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="I118" s="32"/>
+      <c r="J118" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="K118" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="L118" s="31"/>
+      <c r="M118" s="31"/>
+      <c r="N118" s="29">
+        <v>30125371</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B119" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C119" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="D119" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="E119" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="F119" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G119" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="H119" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="I119" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="N119" s="29">
+        <v>29425396</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="31" t="s">
-        <v>147</v>
+        <v>11</v>
       </c>
       <c r="B120" s="31" t="s">
         <v>4</v>
       </c>
       <c r="C120" s="31" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D120" s="31" t="s">
-        <v>146</v>
+        <v>5</v>
       </c>
       <c r="E120" s="31" t="s">
-        <v>145</v>
-      </c>
-      <c r="F120" s="31"/>
+        <v>5</v>
+      </c>
+      <c r="F120" s="31" t="s">
+        <v>5</v>
+      </c>
       <c r="G120" s="31" t="s">
         <v>7</v>
       </c>
       <c r="H120" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="I120" s="32"/>
-      <c r="J120" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="K120" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="L120" s="31"/>
-      <c r="M120" s="31"/>
+        <v>2</v>
+      </c>
+      <c r="I120" s="32" t="s">
+        <v>151</v>
+      </c>
       <c r="N120" s="29">
-        <v>30125371</v>
+        <v>29425396</v>
       </c>
     </row>
     <row r="121" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.2">
@@ -6553,91 +6522,27 @@
         <v>4</v>
       </c>
       <c r="C121" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="D121" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="E121" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="F121" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G121" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="H121" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="I121" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="D121" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="E121" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="F121" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="G121" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="H121" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="I121" s="32" t="s">
-        <v>152</v>
-      </c>
       <c r="N121" s="29">
-        <v>29425396</v>
-      </c>
-    </row>
-    <row r="122" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="B122" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="C122" s="31" t="s">
-        <v>153</v>
-      </c>
-      <c r="D122" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="E122" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="F122" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="G122" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="H122" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="I122" s="32" t="s">
-        <v>152</v>
-      </c>
-      <c r="N122" s="29">
-        <v>29425396</v>
-      </c>
-    </row>
-    <row r="123" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="B123" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="C123" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="D123" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="E123" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="F123" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="G123" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="H123" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="I123" s="32" t="s">
-        <v>152</v>
-      </c>
-      <c r="N123" s="29">
         <v>29425396</v>
       </c>
     </row>

</xml_diff>